<commit_message>
Major revamp of queue and submission guidelines
</commit_message>
<xml_diff>
--- a/docs/IMR-SampleSubmissionSheet_v7(LASTNAME_MMMDD).xlsx
+++ b/docs/IMR-SampleSubmissionSheet_v7(LASTNAME_MMMDD).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="742"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="742" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS (read first)" sheetId="3" r:id="rId1"/>
@@ -1014,7 +1014,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1060,12 +1060,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1250,7 +1244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1311,24 +1305,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1360,44 +1371,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1709,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1840,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,18 +1855,18 @@
       <c r="A2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="25" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1899,41 +1894,41 @@
       <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="33"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="25" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1957,11 +1952,11 @@
       <c r="A16" s="15"/>
     </row>
     <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
     </row>
     <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
@@ -1991,14 +1986,14 @@
       <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
     </row>
     <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="24" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2011,13 +2006,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2040,20 +2035,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -2072,35 +2067,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="J3" s="28" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+      <c r="J3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -2108,35 +2103,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="J4" s="28" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
+      <c r="J4" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -2145,26 +2140,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -2172,30 +2167,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="54"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="54"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -2203,30 +2198,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="54"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -2246,21 +2241,21 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="29"/>
-      <c r="Z8" s="29"/>
-      <c r="AA8" s="29"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
+      <c r="W8" s="54"/>
+      <c r="X8" s="54"/>
+      <c r="Y8" s="54"/>
+      <c r="Z8" s="54"/>
+      <c r="AA8" s="54"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -2272,7 +2267,7 @@
       <c r="C9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="11" t="s">
         <v>42</v>
       </c>
@@ -2284,21 +2279,21 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
-      <c r="Y9" s="29"/>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="29"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="54"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="54"/>
+      <c r="Y9" s="54"/>
+      <c r="Z9" s="54"/>
+      <c r="AA9" s="54"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -2309,7 +2304,7 @@
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="48"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="11" t="s">
         <v>45</v>
       </c>
@@ -2321,21 +2316,21 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -2346,7 +2341,7 @@
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="50"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="11" t="s">
         <v>43</v>
       </c>
@@ -2359,21 +2354,21 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="29"/>
-      <c r="Z11" s="29"/>
-      <c r="AA11" s="29"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="54"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="54"/>
+      <c r="Z11" s="54"/>
+      <c r="AA11" s="54"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -2403,161 +2398,161 @@
       <c r="AF12" s="7"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="33"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="42"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="35"/>
-      <c r="AA14" s="36"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="44"/>
+      <c r="Y14" s="44"/>
+      <c r="Z14" s="44"/>
+      <c r="AA14" s="45"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="35"/>
-      <c r="AA15" s="36"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="44"/>
+      <c r="Y15" s="44"/>
+      <c r="Z15" s="44"/>
+      <c r="AA15" s="45"/>
     </row>
     <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="38"/>
-      <c r="V16" s="38"/>
-      <c r="W16" s="38"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="38"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="39"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="48"/>
     </row>
     <row r="18" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="53"/>
+      <c r="T18" s="53"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
+      <c r="Y18" s="53"/>
+      <c r="Z18" s="53"/>
+      <c r="AA18" s="53"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -3379,35 +3374,35 @@
       <c r="M44" s="10"/>
     </row>
     <row r="45" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="24"/>
-      <c r="O45" s="24"/>
-      <c r="P45" s="24"/>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="24"/>
-      <c r="S45" s="24"/>
-      <c r="T45" s="24"/>
-      <c r="U45" s="24"/>
-      <c r="V45" s="24"/>
-      <c r="W45" s="24"/>
-      <c r="X45" s="24"/>
-      <c r="Y45" s="24"/>
-      <c r="Z45" s="24"/>
-      <c r="AA45" s="24"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53"/>
+      <c r="L45" s="53"/>
+      <c r="M45" s="53"/>
+      <c r="N45" s="53"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="53"/>
+      <c r="R45" s="53"/>
+      <c r="S45" s="53"/>
+      <c r="T45" s="53"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="53"/>
+      <c r="W45" s="53"/>
+      <c r="X45" s="53"/>
+      <c r="Y45" s="53"/>
+      <c r="Z45" s="53"/>
+      <c r="AA45" s="53"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -4162,6 +4157,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A18:AA18"/>
+    <mergeCell ref="A45:AA45"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="M3:AA11"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:AA13"/>
@@ -4173,15 +4177,6 @@
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C14:AA14"/>
-    <mergeCell ref="A18:AA18"/>
-    <mergeCell ref="A45:AA45"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="M3:AA11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4205,20 +4200,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -4237,35 +4232,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="J3" s="28" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+      <c r="J3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -4273,35 +4268,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="J4" s="28" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
+      <c r="J4" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -4310,26 +4305,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -4337,30 +4332,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="54"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="54"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -4368,30 +4363,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="54"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -4406,21 +4401,21 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="29"/>
-      <c r="Z8" s="29"/>
-      <c r="AA8" s="29"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
+      <c r="W8" s="54"/>
+      <c r="X8" s="54"/>
+      <c r="Y8" s="54"/>
+      <c r="Z8" s="54"/>
+      <c r="AA8" s="54"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -4432,27 +4427,27 @@
       <c r="C9" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
-      <c r="Y9" s="29"/>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="29"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="52"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="54"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="54"/>
+      <c r="Y9" s="54"/>
+      <c r="Z9" s="54"/>
+      <c r="AA9" s="54"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -4462,21 +4457,21 @@
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -4489,26 +4484,26 @@
       <c r="C11" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="29"/>
       <c r="H11" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="I11" s="51"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="29"/>
-      <c r="Z11" s="29"/>
-      <c r="AA11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="54"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="54"/>
+      <c r="Z11" s="54"/>
+      <c r="AA11" s="54"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -4542,24 +4537,30 @@
       <c r="C13" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="51"/>
+      <c r="D13" s="29"/>
       <c r="H13" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I13" s="51"/>
+      <c r="I13" s="29"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C15" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="51"/>
+      <c r="D15" s="29"/>
       <c r="H15" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="51"/>
+      <c r="I15" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="M3:AA11"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="D9:I9"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="A7:B7"/>
@@ -4568,12 +4569,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:AA11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4597,20 +4592,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -4629,35 +4624,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="J3" s="28" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+      <c r="J3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -4665,35 +4660,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="J4" s="28" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
+      <c r="J4" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -4702,26 +4697,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -4729,30 +4724,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="54"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="54"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -4760,30 +4755,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="54"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -4798,21 +4793,21 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="29"/>
-      <c r="Z8" s="29"/>
-      <c r="AA8" s="29"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
+      <c r="W8" s="54"/>
+      <c r="X8" s="54"/>
+      <c r="Y8" s="54"/>
+      <c r="Z8" s="54"/>
+      <c r="AA8" s="54"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -4824,25 +4819,25 @@
       <c r="D9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="53"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
-      <c r="Y9" s="29"/>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="29"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="54"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="54"/>
+      <c r="Y9" s="54"/>
+      <c r="Z9" s="54"/>
+      <c r="AA9" s="54"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -4853,25 +4848,25 @@
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="52"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -4888,21 +4883,21 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="29"/>
-      <c r="Z11" s="29"/>
-      <c r="AA11" s="29"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="54"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="54"/>
+      <c r="Z11" s="54"/>
+      <c r="AA11" s="54"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -4931,161 +4926,161 @@
       <c r="AF12" s="7"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="33"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="42"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="35"/>
-      <c r="AA14" s="36"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="44"/>
+      <c r="Y14" s="44"/>
+      <c r="Z14" s="44"/>
+      <c r="AA14" s="45"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="35"/>
-      <c r="AA15" s="36"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="44"/>
+      <c r="Y15" s="44"/>
+      <c r="Z15" s="44"/>
+      <c r="AA15" s="45"/>
     </row>
     <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="38"/>
-      <c r="V16" s="38"/>
-      <c r="W16" s="38"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="38"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="39"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="48"/>
     </row>
     <row r="18" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="53"/>
+      <c r="T18" s="53"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
+      <c r="Y18" s="53"/>
+      <c r="Z18" s="53"/>
+      <c r="AA18" s="53"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -5884,35 +5879,35 @@
       <c r="J42" s="20"/>
     </row>
     <row r="45" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="24"/>
-      <c r="O45" s="24"/>
-      <c r="P45" s="24"/>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="24"/>
-      <c r="S45" s="24"/>
-      <c r="T45" s="24"/>
-      <c r="U45" s="24"/>
-      <c r="V45" s="24"/>
-      <c r="W45" s="24"/>
-      <c r="X45" s="24"/>
-      <c r="Y45" s="24"/>
-      <c r="Z45" s="24"/>
-      <c r="AA45" s="24"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53"/>
+      <c r="L45" s="53"/>
+      <c r="M45" s="53"/>
+      <c r="N45" s="53"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="53"/>
+      <c r="R45" s="53"/>
+      <c r="S45" s="53"/>
+      <c r="T45" s="53"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="53"/>
+      <c r="W45" s="53"/>
+      <c r="X45" s="53"/>
+      <c r="Y45" s="53"/>
+      <c r="Z45" s="53"/>
+      <c r="AA45" s="53"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -6659,6 +6654,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:AA11"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="C15:AA15"/>
     <mergeCell ref="C16:AA16"/>
     <mergeCell ref="A18:AA18"/>
@@ -6669,16 +6674,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:AA13"/>
     <mergeCell ref="C14:AA14"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:AA11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -6702,20 +6697,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -6731,32 +6726,32 @@
       <c r="AC2" s="7"/>
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="J3" s="28" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+      <c r="J3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
@@ -6764,32 +6759,32 @@
       <c r="AC3" s="7"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="J4" s="28" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
+      <c r="J4" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
@@ -6798,21 +6793,21 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="54"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
@@ -6820,27 +6815,27 @@
       <c r="AC5" s="7"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
@@ -6848,27 +6843,27 @@
       <c r="AC6" s="7"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="7"/>
@@ -6883,18 +6878,18 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
+      <c r="W8" s="54"/>
+      <c r="X8" s="54"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
@@ -6906,22 +6901,22 @@
       <c r="D9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="53"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="54"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="54"/>
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="7"/>
@@ -6932,22 +6927,22 @@
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="52"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="7"/>
@@ -6964,18 +6959,18 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="54"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="54"/>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
@@ -7001,144 +6996,144 @@
       <c r="AC12" s="7"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="33"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="42"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="36"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="45"/>
     </row>
     <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="38"/>
-      <c r="U15" s="38"/>
-      <c r="V15" s="38"/>
-      <c r="W15" s="38"/>
-      <c r="X15" s="39"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="48"/>
     </row>
     <row r="17" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57" t="s">
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57" t="s">
+      <c r="H17" s="58"/>
+      <c r="I17" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="J17" s="57"/>
-      <c r="K17" s="56" t="s">
+      <c r="J17" s="58"/>
+      <c r="K17" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="L17" s="57" t="s">
+      <c r="L17" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="M17" s="57"/>
-      <c r="N17" s="58" t="s">
+      <c r="M17" s="58"/>
+      <c r="N17" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="O17" s="58"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="58"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="58"/>
-      <c r="U17" s="58"/>
-      <c r="V17" s="58"/>
-      <c r="W17" s="58"/>
-      <c r="X17" s="58"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>1</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
       <c r="N18" s="55"/>
       <c r="O18" s="55"/>
       <c r="P18" s="55"/>
@@ -7155,16 +7150,16 @@
       <c r="B19" s="10">
         <v>2</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
       <c r="N19" s="55"/>
       <c r="O19" s="55"/>
       <c r="P19" s="55"/>
@@ -7181,16 +7176,16 @@
       <c r="B20" s="10">
         <v>3</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
       <c r="N20" s="55"/>
       <c r="O20" s="55"/>
       <c r="P20" s="55"/>
@@ -7207,16 +7202,16 @@
       <c r="B21" s="10">
         <v>4</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
       <c r="N21" s="55"/>
       <c r="O21" s="55"/>
       <c r="P21" s="55"/>
@@ -7233,16 +7228,16 @@
       <c r="B22" s="10">
         <v>5</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
       <c r="N22" s="55"/>
       <c r="O22" s="55"/>
       <c r="P22" s="55"/>
@@ -7259,16 +7254,16 @@
       <c r="B23" s="10">
         <v>6</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
       <c r="N23" s="55"/>
       <c r="O23" s="55"/>
       <c r="P23" s="55"/>
@@ -7285,16 +7280,16 @@
       <c r="B24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
       <c r="N24" s="55"/>
       <c r="O24" s="55"/>
       <c r="P24" s="55"/>
@@ -7309,14 +7304,40 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="N23:X23"/>
-    <mergeCell ref="N24:X24"/>
-    <mergeCell ref="N17:X17"/>
-    <mergeCell ref="N18:X18"/>
-    <mergeCell ref="N19:X19"/>
-    <mergeCell ref="N20:X20"/>
-    <mergeCell ref="N21:X21"/>
-    <mergeCell ref="N22:X22"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:X11"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C14:X14"/>
+    <mergeCell ref="C15:X15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C13:X13"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="L18:M18"/>
@@ -7332,40 +7353,14 @@
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C14:X14"/>
-    <mergeCell ref="C15:X15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C13:X13"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:X11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="N23:X23"/>
+    <mergeCell ref="N24:X24"/>
+    <mergeCell ref="N17:X17"/>
+    <mergeCell ref="N18:X18"/>
+    <mergeCell ref="N19:X19"/>
+    <mergeCell ref="N20:X20"/>
+    <mergeCell ref="N21:X21"/>
+    <mergeCell ref="N22:X22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>